<commit_message>
Setup anatomy, subanatomy, findings, location, laterality, char etc.
</commit_message>
<xml_diff>
--- a/Chest Findings Reicher Wu 1_9_2018.xlsx
+++ b/Chest Findings Reicher Wu 1_9_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadeem.ansari@ibm.com/Documents/Annotation-App/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadeem.ansari@ibm.com/Documents/Annotation-App-v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3902,11 +3902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K336"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A329" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G309" sqref="G309"/>
     </sheetView>
   </sheetViews>
@@ -3961,7 +3960,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3996,7 +3995,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -4031,7 +4030,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -4066,7 +4065,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -4101,7 +4100,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -4136,7 +4135,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -4171,7 +4170,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -4206,7 +4205,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -4241,7 +4240,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -4276,7 +4275,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -4311,7 +4310,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -4346,7 +4345,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -4381,7 +4380,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -4416,7 +4415,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -4451,7 +4450,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -4486,7 +4485,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -4521,7 +4520,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -4556,7 +4555,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -4591,7 +4590,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -4626,7 +4625,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -4661,7 +4660,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -4696,7 +4695,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -4731,7 +4730,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -4766,7 +4765,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -4801,7 +4800,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -4836,7 +4835,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -4871,7 +4870,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -4906,7 +4905,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -4941,7 +4940,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -4976,7 +4975,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -5011,7 +5010,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -5046,7 +5045,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -5081,7 +5080,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -5116,7 +5115,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -5151,7 +5150,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -5186,7 +5185,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -5221,7 +5220,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -5256,7 +5255,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -5291,7 +5290,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -5326,7 +5325,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -5361,7 +5360,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -5396,7 +5395,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -5431,7 +5430,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -5466,7 +5465,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="70.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="70.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -5501,7 +5500,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="70.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="70.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -5536,7 +5535,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -5571,7 +5570,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -5606,7 +5605,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -5641,7 +5640,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -5676,7 +5675,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -5711,7 +5710,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -5746,7 +5745,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
@@ -5781,7 +5780,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -5816,7 +5815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -5851,7 +5850,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
@@ -5886,7 +5885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -5921,7 +5920,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -5956,7 +5955,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -5991,7 +5990,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -6026,7 +6025,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -6061,7 +6060,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -6096,7 +6095,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
@@ -6131,7 +6130,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -6166,7 +6165,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
@@ -6201,7 +6200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
@@ -6236,7 +6235,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -6271,7 +6270,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
@@ -6306,7 +6305,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
@@ -6341,7 +6340,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
@@ -6376,7 +6375,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
@@ -6411,7 +6410,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
@@ -6446,7 +6445,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -6481,7 +6480,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
@@ -6516,7 +6515,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
@@ -6551,7 +6550,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
@@ -6586,7 +6585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
@@ -6621,7 +6620,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
@@ -6656,7 +6655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
@@ -6691,7 +6690,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
@@ -6726,7 +6725,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
@@ -6761,7 +6760,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>0</v>
       </c>
@@ -6796,7 +6795,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>0</v>
       </c>
@@ -6831,7 +6830,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
@@ -6866,7 +6865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>0</v>
       </c>
@@ -6901,7 +6900,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>0</v>
       </c>
@@ -6936,7 +6935,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>0</v>
       </c>
@@ -6971,7 +6970,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>0</v>
       </c>
@@ -7006,7 +7005,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>0</v>
       </c>
@@ -7041,7 +7040,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>0</v>
       </c>
@@ -7076,7 +7075,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>0</v>
       </c>
@@ -7111,7 +7110,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>0</v>
       </c>
@@ -7146,7 +7145,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>0</v>
       </c>
@@ -7181,7 +7180,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>0</v>
       </c>
@@ -7216,7 +7215,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>0</v>
       </c>
@@ -7251,7 +7250,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>0</v>
       </c>
@@ -7286,7 +7285,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>0</v>
       </c>
@@ -7321,7 +7320,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>0</v>
       </c>
@@ -7356,7 +7355,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>0</v>
       </c>
@@ -7391,7 +7390,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>0</v>
       </c>
@@ -7426,7 +7425,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>0</v>
       </c>
@@ -7461,7 +7460,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>0</v>
       </c>
@@ -7496,7 +7495,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>0</v>
       </c>
@@ -7531,7 +7530,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>0</v>
       </c>
@@ -7566,7 +7565,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>0</v>
       </c>
@@ -7601,7 +7600,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>0</v>
       </c>
@@ -7636,7 +7635,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>0</v>
       </c>
@@ -7671,7 +7670,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>0</v>
       </c>
@@ -7706,7 +7705,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>0</v>
       </c>
@@ -7741,7 +7740,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>0</v>
       </c>
@@ -7776,7 +7775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>1</v>
       </c>
@@ -7811,7 +7810,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>1</v>
       </c>
@@ -7846,7 +7845,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>1</v>
       </c>
@@ -7881,7 +7880,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>1</v>
       </c>
@@ -7916,7 +7915,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>1</v>
       </c>
@@ -7951,7 +7950,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>1</v>
       </c>
@@ -7986,7 +7985,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>1</v>
       </c>
@@ -8021,7 +8020,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>1</v>
       </c>
@@ -8056,7 +8055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>1</v>
       </c>
@@ -8091,7 +8090,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>1</v>
       </c>
@@ -8126,7 +8125,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>1</v>
       </c>
@@ -8161,7 +8160,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>1</v>
       </c>
@@ -8196,7 +8195,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>1</v>
       </c>
@@ -8231,7 +8230,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>1</v>
       </c>
@@ -8266,7 +8265,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>1</v>
       </c>
@@ -8301,7 +8300,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>1</v>
       </c>
@@ -8336,7 +8335,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>1</v>
       </c>
@@ -8371,7 +8370,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>1</v>
       </c>
@@ -8406,7 +8405,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>1</v>
       </c>
@@ -8441,7 +8440,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>1</v>
       </c>
@@ -8476,7 +8475,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>1</v>
       </c>
@@ -8511,7 +8510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>1</v>
       </c>
@@ -8546,7 +8545,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>1</v>
       </c>
@@ -8581,7 +8580,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>1</v>
       </c>
@@ -8616,7 +8615,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>1</v>
       </c>
@@ -8651,7 +8650,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>1</v>
       </c>
@@ -8686,7 +8685,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>1</v>
       </c>
@@ -8721,7 +8720,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>209</v>
       </c>
@@ -8756,7 +8755,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>209</v>
       </c>
@@ -8791,7 +8790,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>209</v>
       </c>
@@ -8826,7 +8825,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>209</v>
       </c>
@@ -8861,7 +8860,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>209</v>
       </c>
@@ -8896,7 +8895,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>209</v>
       </c>
@@ -8931,7 +8930,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="44.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>209</v>
       </c>
@@ -8966,7 +8965,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="46.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>209</v>
       </c>
@@ -9001,7 +9000,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>2</v>
       </c>
@@ -9036,7 +9035,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>2</v>
       </c>
@@ -9071,7 +9070,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>2</v>
       </c>
@@ -9106,7 +9105,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>2</v>
       </c>
@@ -9141,7 +9140,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>2</v>
       </c>
@@ -9176,7 +9175,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>2</v>
       </c>
@@ -9211,7 +9210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>2</v>
       </c>
@@ -9246,7 +9245,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>2</v>
       </c>
@@ -9281,7 +9280,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>2</v>
       </c>
@@ -9316,7 +9315,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>2</v>
       </c>
@@ -9351,7 +9350,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>2</v>
       </c>
@@ -9386,7 +9385,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="45.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" ht="45.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>2</v>
       </c>
@@ -9421,7 +9420,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>2</v>
       </c>
@@ -9456,7 +9455,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>2</v>
       </c>
@@ -9491,7 +9490,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>2</v>
       </c>
@@ -9526,7 +9525,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>2</v>
       </c>
@@ -9561,7 +9560,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>2</v>
       </c>
@@ -9596,7 +9595,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>2</v>
       </c>
@@ -9631,7 +9630,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>2</v>
       </c>
@@ -9666,7 +9665,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>2</v>
       </c>
@@ -9701,7 +9700,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="44.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>2</v>
       </c>
@@ -9736,7 +9735,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>2</v>
       </c>
@@ -9771,7 +9770,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>2</v>
       </c>
@@ -9806,7 +9805,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>2</v>
       </c>
@@ -9841,7 +9840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>2</v>
       </c>
@@ -9876,7 +9875,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>2</v>
       </c>
@@ -9911,7 +9910,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="172" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>2</v>
       </c>
@@ -9946,7 +9945,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>2</v>
       </c>
@@ -9981,7 +9980,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>2</v>
       </c>
@@ -10016,7 +10015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="175" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>2</v>
       </c>
@@ -10051,7 +10050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>2</v>
       </c>
@@ -10086,7 +10085,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>2</v>
       </c>
@@ -10121,7 +10120,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="178" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>2</v>
       </c>
@@ -10156,7 +10155,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>3</v>
       </c>
@@ -10191,7 +10190,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>3</v>
       </c>
@@ -10226,7 +10225,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>3</v>
       </c>
@@ -10261,7 +10260,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>3</v>
       </c>
@@ -10296,7 +10295,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>3</v>
       </c>
@@ -10331,7 +10330,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="184" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>3</v>
       </c>
@@ -10366,7 +10365,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="185" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>3</v>
       </c>
@@ -10401,7 +10400,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="186" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>3</v>
       </c>
@@ -10436,7 +10435,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="187" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>3</v>
       </c>
@@ -10471,7 +10470,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="188" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>3</v>
       </c>
@@ -10506,7 +10505,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="189" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>3</v>
       </c>
@@ -10541,7 +10540,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="190" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>3</v>
       </c>
@@ -10576,7 +10575,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="191" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>3</v>
       </c>
@@ -10611,7 +10610,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="192" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>3</v>
       </c>
@@ -10646,7 +10645,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>3</v>
       </c>
@@ -10681,7 +10680,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="194" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>3</v>
       </c>
@@ -10716,7 +10715,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="195" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>3</v>
       </c>
@@ -10751,7 +10750,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="196" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>3</v>
       </c>
@@ -10786,7 +10785,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="197" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>3</v>
       </c>
@@ -10821,7 +10820,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="198" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>3</v>
       </c>
@@ -10856,7 +10855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>3</v>
       </c>
@@ -10891,7 +10890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>3</v>
       </c>
@@ -10926,7 +10925,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>3</v>
       </c>
@@ -10961,7 +10960,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>3</v>
       </c>
@@ -10996,7 +10995,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>3</v>
       </c>
@@ -11031,7 +11030,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>3</v>
       </c>
@@ -11066,7 +11065,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>3</v>
       </c>
@@ -11101,7 +11100,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>3</v>
       </c>
@@ -11136,7 +11135,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>3</v>
       </c>
@@ -11171,7 +11170,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>3</v>
       </c>
@@ -11206,7 +11205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>3</v>
       </c>
@@ -11241,7 +11240,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>3</v>
       </c>
@@ -11276,7 +11275,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>3</v>
       </c>
@@ -11311,7 +11310,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>3</v>
       </c>
@@ -11346,7 +11345,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>3</v>
       </c>
@@ -11381,7 +11380,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="214" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>3</v>
       </c>
@@ -11416,7 +11415,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="215" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>3</v>
       </c>
@@ -11451,7 +11450,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="216" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>3</v>
       </c>
@@ -11486,7 +11485,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="217" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>3</v>
       </c>
@@ -11521,7 +11520,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="218" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>3</v>
       </c>
@@ -11556,7 +11555,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="219" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>3</v>
       </c>
@@ -11591,7 +11590,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="220" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>3</v>
       </c>
@@ -11626,7 +11625,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="221" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>3</v>
       </c>
@@ -11661,7 +11660,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="222" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>3</v>
       </c>
@@ -11696,7 +11695,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="223" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>3</v>
       </c>
@@ -11731,7 +11730,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="224" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>3</v>
       </c>
@@ -11766,7 +11765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="225" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>3</v>
       </c>
@@ -11801,7 +11800,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="226" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>3</v>
       </c>
@@ -11836,7 +11835,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="227" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>3</v>
       </c>
@@ -11871,7 +11870,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="228" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>3</v>
       </c>
@@ -11906,7 +11905,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="229" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>3</v>
       </c>
@@ -11941,7 +11940,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="230" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>4</v>
       </c>
@@ -11976,7 +11975,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="231" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>4</v>
       </c>
@@ -12011,7 +12010,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="232" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>4</v>
       </c>
@@ -12046,7 +12045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="233" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>4</v>
       </c>
@@ -12081,7 +12080,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="234" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>4</v>
       </c>
@@ -12116,7 +12115,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="235" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>4</v>
       </c>
@@ -12151,7 +12150,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="236" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>4</v>
       </c>
@@ -12186,7 +12185,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="237" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>4</v>
       </c>
@@ -12221,7 +12220,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="238" spans="1:11" ht="44.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:11" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>4</v>
       </c>
@@ -12256,7 +12255,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="239" spans="1:11" ht="42.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:11" ht="42.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>4</v>
       </c>
@@ -12291,7 +12290,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="240" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>4</v>
       </c>
@@ -12326,7 +12325,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="241" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>4</v>
       </c>
@@ -12361,7 +12360,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="242" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>4</v>
       </c>
@@ -12396,7 +12395,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="243" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>4</v>
       </c>
@@ -12431,7 +12430,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="244" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>4</v>
       </c>
@@ -12466,7 +12465,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="245" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>4</v>
       </c>
@@ -12501,7 +12500,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="246" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>4</v>
       </c>
@@ -12536,7 +12535,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="247" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>4</v>
       </c>
@@ -12571,7 +12570,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="248" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>4</v>
       </c>
@@ -12606,7 +12605,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="249" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>4</v>
       </c>
@@ -12641,7 +12640,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="250" spans="1:11" ht="44.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:11" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>4</v>
       </c>
@@ -12676,7 +12675,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="251" spans="1:11" ht="42.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11" ht="42.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
         <v>4</v>
       </c>
@@ -12711,7 +12710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="252" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>4</v>
       </c>
@@ -12746,7 +12745,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="253" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>4</v>
       </c>
@@ -12781,7 +12780,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="254" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>4</v>
       </c>
@@ -12816,7 +12815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="255" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>4</v>
       </c>
@@ -12851,7 +12850,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="256" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>4</v>
       </c>
@@ -12886,7 +12885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="257" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
         <v>4</v>
       </c>
@@ -12921,7 +12920,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="258" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
         <v>4</v>
       </c>
@@ -12956,7 +12955,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="259" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>4</v>
       </c>
@@ -12991,7 +12990,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="260" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
         <v>4</v>
       </c>
@@ -13026,7 +13025,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="261" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>4</v>
       </c>
@@ -13061,7 +13060,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="262" spans="1:11" ht="44.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:11" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
         <v>4</v>
       </c>
@@ -13096,7 +13095,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="263" spans="1:11" ht="42.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:11" ht="42.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>4</v>
       </c>
@@ -13131,7 +13130,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="264" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>4</v>
       </c>
@@ -13166,7 +13165,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="265" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>4</v>
       </c>
@@ -13201,7 +13200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="266" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>4</v>
       </c>
@@ -13236,7 +13235,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="267" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
         <v>4</v>
       </c>
@@ -13271,7 +13270,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="268" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>4</v>
       </c>
@@ -13306,7 +13305,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="269" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>4</v>
       </c>
@@ -13341,7 +13340,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="270" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
         <v>4</v>
       </c>
@@ -13376,7 +13375,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="271" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
         <v>4</v>
       </c>
@@ -13411,7 +13410,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="272" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
         <v>4</v>
       </c>
@@ -13446,7 +13445,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="273" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
         <v>4</v>
       </c>
@@ -13481,7 +13480,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="274" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>4</v>
       </c>
@@ -13516,7 +13515,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="275" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
         <v>4</v>
       </c>
@@ -13551,7 +13550,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="276" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>4</v>
       </c>
@@ -13586,7 +13585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="277" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
         <v>4</v>
       </c>
@@ -13621,7 +13620,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="278" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>4</v>
       </c>
@@ -13656,7 +13655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="279" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
         <v>4</v>
       </c>
@@ -15655,13 +15654,7 @@
       <c r="D336" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K335">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Other"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K335"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>